<commit_message>
Changes, Edited Datadictionary, Added Modeldictionary
</commit_message>
<xml_diff>
--- a/KT1/KT1.2/KT1.2.1 Globale Planning/Globale Planning v1.0.0.xlsx
+++ b/KT1/KT1.2/KT1.2.1 Globale Planning/Globale Planning v1.0.0.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenley Strik\Documents\GitKraken\Periode_11_Proef_PVB_Tim_Kenley\Periode_11_Proef_PVB_Tim_Kenley\KT1\KT1.2\KT1.2.1 Globale Planning\"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="87">
   <si>
     <t>Globale Planning</t>
   </si>
@@ -311,11 +311,14 @@
   <si>
     <t>↓</t>
   </si>
+  <si>
+    <t>1,5 uur</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1643,7 +1646,7 @@
   <dimension ref="A1:L102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2154,7 +2157,7 @@
         <v>20</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G33" s="8"/>
     </row>
@@ -2215,9 +2218,11 @@
       </c>
       <c r="D37" s="16"/>
       <c r="E37" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="F37" s="16"/>
+        <v>86</v>
+      </c>
+      <c r="F37" s="16" t="s">
+        <v>24</v>
+      </c>
       <c r="G37" s="8"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -2227,8 +2232,12 @@
         <v>42</v>
       </c>
       <c r="D38" s="16"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="16"/>
+      <c r="E38" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="F38" s="16" t="s">
+        <v>24</v>
+      </c>
       <c r="G38" s="8"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -2238,8 +2247,12 @@
         <v>43</v>
       </c>
       <c r="D39" s="16"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="16"/>
+      <c r="E39" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="F39" s="16" t="s">
+        <v>23</v>
+      </c>
       <c r="G39" s="8"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -2249,8 +2262,12 @@
         <v>44</v>
       </c>
       <c r="D40" s="16"/>
-      <c r="E40" s="16"/>
-      <c r="F40" s="16"/>
+      <c r="E40" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="F40" s="16" t="s">
+        <v>23</v>
+      </c>
       <c r="G40" s="8"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>